<commit_message>
Implementation revisions to budget by model number and modify model output written to Excel (i.e. oh, rates, asset info, formulas vs hard code)
</commit_message>
<xml_diff>
--- a/model_inputs/budget_report_input.xlsx
+++ b/model_inputs/budget_report_input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jjc92\Downloads\biomed-service-delivery-cost-model\model_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC8E07E-660C-4CF2-8261-0E234B155F2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40B404C0-5D27-4757-B0F6-C7DAE4750DE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="1076">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="1079">
   <si>
     <t>asset_description</t>
   </si>
@@ -3275,6 +3275,15 @@
   </si>
   <si>
     <t>Shop Code List</t>
+  </si>
+  <si>
+    <t>model_num</t>
+  </si>
+  <si>
+    <t>CRIR348CL</t>
+  </si>
+  <si>
+    <t>08257869</t>
   </si>
 </sst>
 </file>
@@ -3413,10 +3422,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{04025D63-520A-40A9-99FC-2851D2951CE8}" name="Table1" displayName="Table1" ref="A1:E1000" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:E1000" xr:uid="{EC1C5615-35A0-4672-9ED1-C04070F7D11B}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{177FCAFB-B451-4AD7-B0F8-A10928CF2710}" name="asset_description"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{04025D63-520A-40A9-99FC-2851D2951CE8}" name="Table1" displayName="Table1" ref="A1:F1000" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:F1000" xr:uid="{EC1C5615-35A0-4672-9ED1-C04070F7D11B}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{177FCAFB-B451-4AD7-B0F8-A10928CF2710}" name="model_num"/>
+    <tableColumn id="6" xr3:uid="{1E6C6204-DF0D-4154-9940-B0C5258AEF4D}" name="asset_description"/>
     <tableColumn id="2" xr3:uid="{6B329163-C91C-4AF1-9972-F42067124B8E}" name="quantity"/>
     <tableColumn id="3" xr3:uid="{24CE629B-E37A-485C-8556-0A3E6BC1B761}" name="health_auth"/>
     <tableColumn id="4" xr3:uid="{9391C880-CCD7-47F0-BD57-864178EEF41F}" name="site_code"/>
@@ -3700,115 +3710,91 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="89.5703125" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" customWidth="1"/>
+    <col min="2" max="2" width="89.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>533</v>
-      </c>
-      <c r="B2">
+        <v>1077</v>
+      </c>
+      <c r="B2" t="s">
+        <v>904</v>
+      </c>
+      <c r="C2">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>1072</v>
-      </c>
       <c r="D2" t="s">
-        <v>926</v>
+        <v>1073</v>
       </c>
       <c r="E2" t="s">
-        <v>1055</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1017</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>533</v>
-      </c>
-      <c r="B3">
+        <v>1078</v>
+      </c>
+      <c r="B3" t="s">
+        <v>633</v>
+      </c>
+      <c r="C3">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
-        <v>1072</v>
-      </c>
       <c r="D3" t="s">
-        <v>929</v>
+        <v>1073</v>
       </c>
       <c r="E3" t="s">
-        <v>1063</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>533</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1072</v>
-      </c>
-      <c r="D4" t="s">
-        <v>933</v>
-      </c>
-      <c r="E4" t="s">
-        <v>1062</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>533</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>1072</v>
-      </c>
-      <c r="D5" t="s">
-        <v>936</v>
-      </c>
-      <c r="E5" t="s">
-        <v>1064</v>
+        <v>1021</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1057</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1000" xr:uid="{A6666E27-895A-4F00-96C7-8175F7CD4756}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1000" xr:uid="{A6666E27-895A-4F00-96C7-8175F7CD4756}">
       <formula1>HealthAuth</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1000" xr:uid="{4099E842-885D-459F-BEFF-0BFB5ED168A2}">
-      <formula1>INDIRECT(C2)</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E8:E1000 E2:E6" xr:uid="{4099E842-885D-459F-BEFF-0BFB5ED168A2}">
+      <formula1>INDIRECT(D2)</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1000" xr:uid="{B8F6451C-BE14-41EC-BC0C-18409E093CA3}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1000" xr:uid="{B8F6451C-BE14-41EC-BC0C-18409E093CA3}">
       <formula1>1</formula1>
       <formula2>999999</formula2>
     </dataValidation>
@@ -3821,17 +3807,17 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A2CD70B7-AEE2-49C8-920A-3C6591F9BE9B}">
+          <x14:formula1>
+            <xm:f>'Shop Code List'!$A$2:$A$23</xm:f>
+          </x14:formula1>
+          <xm:sqref>F8:F1000 F2:F6</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0D7A4FCF-CDE2-45CA-A76C-3147252C0376}">
           <x14:formula1>
             <xm:f>'Assets List'!$A$2:$A$916</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A1000</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A2CD70B7-AEE2-49C8-920A-3C6591F9BE9B}">
-          <x14:formula1>
-            <xm:f>'Shop Code List'!$A$2:$A$23</xm:f>
-          </x14:formula1>
-          <xm:sqref>E2:E1000</xm:sqref>
+          <xm:sqref>A19:B1000 B2:B6 B8:B18</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3845,7 +3831,7 @@
   <dimension ref="A1:A916"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9067,7 +9053,7 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixed bugs and added print statements to console output
</commit_message>
<xml_diff>
--- a/model_inputs/budget_report_input.xlsx
+++ b/model_inputs/budget_report_input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jjc92\Downloads\biomed-service-delivery-cost-model\model_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40B404C0-5D27-4757-B0F6-C7DAE4750DE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD22B7D-A5D0-4BC7-9866-6225685335A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="1079">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1089" uniqueCount="1078">
   <si>
     <t>asset_description</t>
   </si>
@@ -3280,10 +3280,7 @@
     <t>model_num</t>
   </si>
   <si>
-    <t>CRIR348CL</t>
-  </si>
-  <si>
-    <t>08257869</t>
+    <t>012378</t>
   </si>
 </sst>
 </file>
@@ -3710,10 +3707,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:F284"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3751,51 +3748,31 @@
         <v>1077</v>
       </c>
       <c r="B2" t="s">
-        <v>904</v>
+        <v>249</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>1073</v>
+        <v>1074</v>
       </c>
       <c r="E2" t="s">
-        <v>1017</v>
+        <v>1045</v>
       </c>
       <c r="F2" t="s">
-        <v>1057</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1078</v>
-      </c>
-      <c r="B3" t="s">
-        <v>633</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1073</v>
-      </c>
-      <c r="E3" t="s">
-        <v>1021</v>
-      </c>
-      <c r="F3" t="s">
-        <v>1057</v>
+        <v>1065</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E6 E8:E997" xr:uid="{4099E842-885D-459F-BEFF-0BFB5ED168A2}">
+      <formula1>INDIRECT(D2)</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1000" xr:uid="{A6666E27-895A-4F00-96C7-8175F7CD4756}">
       <formula1>HealthAuth</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E8:E1000 E2:E6" xr:uid="{4099E842-885D-459F-BEFF-0BFB5ED168A2}">
-      <formula1>INDIRECT(D2)</formula1>
-    </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1000" xr:uid="{B8F6451C-BE14-41EC-BC0C-18409E093CA3}">
-      <formula1>1</formula1>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{2139FE40-EBEC-4A4A-B1C4-B5F27799EDB8}">
+      <formula1>-999999</formula1>
       <formula2>999999</formula2>
     </dataValidation>
   </dataValidations>
@@ -3811,13 +3788,13 @@
           <x14:formula1>
             <xm:f>'Shop Code List'!$A$2:$A$23</xm:f>
           </x14:formula1>
-          <xm:sqref>F8:F1000 F2:F6</xm:sqref>
+          <xm:sqref>F2:F6 F8:F997</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0D7A4FCF-CDE2-45CA-A76C-3147252C0376}">
           <x14:formula1>
             <xm:f>'Assets List'!$A$2:$A$916</xm:f>
           </x14:formula1>
-          <xm:sqref>A19:B1000 B2:B6 B8:B18</xm:sqref>
+          <xm:sqref>B2:B6 B8:B18 A19:B997</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -8478,7 +8455,7 @@
   <dimension ref="A1:D75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Modified output to include service contract cost field for imaging devices
</commit_message>
<xml_diff>
--- a/model_inputs/budget_report_input.xlsx
+++ b/model_inputs/budget_report_input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jjc92\Downloads\biomed-service-delivery-cost-model\model_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD22B7D-A5D0-4BC7-9866-6225685335A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{222A433B-9FF8-4E27-82F0-4DBFAF3A1156}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1089" uniqueCount="1078">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1102" uniqueCount="1079">
   <si>
     <t>asset_description</t>
   </si>
@@ -3281,13 +3281,16 @@
   </si>
   <si>
     <t>012378</t>
+  </si>
+  <si>
+    <t>012379</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3299,6 +3302,12 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3707,10 +3716,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:F284"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3763,9 +3772,70 @@
         <v>1065</v>
       </c>
     </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1078</v>
+      </c>
+      <c r="B3" t="s">
+        <v>249</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1074</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1045</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1074</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1045</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1074</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1045</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1057</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E6 E8:E997" xr:uid="{4099E842-885D-459F-BEFF-0BFB5ED168A2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E8:E997 E2:E6" xr:uid="{4099E842-885D-459F-BEFF-0BFB5ED168A2}">
       <formula1>INDIRECT(D2)</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1000" xr:uid="{A6666E27-895A-4F00-96C7-8175F7CD4756}">
@@ -3788,13 +3858,13 @@
           <x14:formula1>
             <xm:f>'Shop Code List'!$A$2:$A$23</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F6 F8:F997</xm:sqref>
+          <xm:sqref>F8:F997 F2:F6</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0D7A4FCF-CDE2-45CA-A76C-3147252C0376}">
           <x14:formula1>
             <xm:f>'Assets List'!$A$2:$A$916</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B6 B8:B18 A19:B997</xm:sqref>
+          <xm:sqref>A19:B997 B8:B18 B2:B6</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Added docstrings and in-line comments to everything
</commit_message>
<xml_diff>
--- a/model_inputs/budget_report_input.xlsx
+++ b/model_inputs/budget_report_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jjc92\Downloads\biomed-service-delivery-cost-model\model_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{222A433B-9FF8-4E27-82F0-4DBFAF3A1156}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{258348C7-D8E1-48C5-A1F4-FBD322D2D0CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3585" yWindow="3585" windowWidth="21600" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User Input" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1102" uniqueCount="1079">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1106" uniqueCount="1079">
   <si>
     <t>asset_description</t>
   </si>
@@ -3716,10 +3716,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3829,6 +3829,26 @@
         <v>1045</v>
       </c>
       <c r="F5" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1074</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1045</v>
+      </c>
+      <c r="F6" t="s">
         <v>1057</v>
       </c>
     </row>

</xml_diff>